<commit_message>
State machine spreadsheet update
</commit_message>
<xml_diff>
--- a/ideas/stateMachine.xlsx
+++ b/ideas/stateMachine.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="52700" yWindow="1340" windowWidth="22540" windowHeight="18980" tabRatio="161"/>
+    <workbookView xWindow="52695" yWindow="1335" windowWidth="22545" windowHeight="13740" tabRatio="243"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Legend" sheetId="2" r:id="rId1"/>
+    <sheet name="Algorithm" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$F$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Algorithm!$A$2:$F$35</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Prev</t>
   </si>
@@ -181,13 +182,79 @@
   </si>
   <si>
     <t>U-&gt;arm motor,  U-&gt; conveyor, Stop-&gt; liftmotor</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Arm</t>
+  </si>
+  <si>
+    <t>Conveyor</t>
+  </si>
+  <si>
+    <t>Lift</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Picking up</t>
+  </si>
+  <si>
+    <t>Dropping off</t>
+  </si>
+  <si>
+    <t>Loading</t>
+  </si>
+  <si>
+    <t>Unloading</t>
+  </si>
+  <si>
+    <t>Stopped</t>
+  </si>
+  <si>
+    <t>Up Moving</t>
+  </si>
+  <si>
+    <t>Down Moving</t>
+  </si>
+  <si>
+    <t>Lift Reaches Position</t>
+  </si>
+  <si>
+    <t>Arm Stops</t>
+  </si>
+  <si>
+    <t>Load a Tote</t>
+  </si>
+  <si>
+    <t>State Transitions</t>
+  </si>
+  <si>
+    <t>Unload a Tote</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>Stop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -195,6 +262,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -277,18 +351,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -614,20 +694,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" thickBot="1"/>
-    <row r="2" spans="1:6" ht="13" thickBot="1">
+    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -643,7 +868,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -663,7 +888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -675,7 +900,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -687,7 +912,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -695,7 +920,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -715,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -727,7 +952,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -739,7 +964,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -747,7 +972,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -767,7 +992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>9</v>
@@ -779,7 +1004,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -791,7 +1016,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -809,7 +1034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>30</v>
@@ -821,7 +1046,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
@@ -833,7 +1058,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -851,7 +1076,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>39</v>
@@ -863,7 +1088,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>41</v>
@@ -875,7 +1100,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>43</v>
@@ -893,7 +1118,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>46</v>
@@ -905,7 +1130,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>47</v>
@@ -917,7 +1142,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -925,7 +1150,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -945,7 +1170,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>23</v>
@@ -957,7 +1182,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -969,7 +1194,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>26</v>
@@ -987,7 +1212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>31</v>
@@ -999,7 +1224,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -1011,7 +1236,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>13</v>
@@ -1029,7 +1254,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>16</v>
@@ -1041,7 +1266,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>18</v>
@@ -1053,7 +1278,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>35</v>
@@ -1071,7 +1296,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>40</v>
@@ -1083,7 +1308,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="13" thickBot="1">
+    <row r="35" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>42</v>

</xml_diff>